<commit_message>
added covered call -- updated driver.py
</commit_message>
<xml_diff>
--- a/CRSRTrackingGrid.xlsx
+++ b/CRSRTrackingGrid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reiner/Desktop/Python/CRSR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477459B8-F033-D345-80F3-407B06E01964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BB90CD-1787-BD4B-A33D-282CCC9FDD6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14460" activeTab="1" xr2:uid="{CF0064EA-4A03-6541-A4B0-E1A1F77CAE04}"/>
   </bookViews>
   <sheets>
     <sheet name="CRSRShares" sheetId="1" r:id="rId1"/>
@@ -422,7 +422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A445721-F1D6-914D-B3EC-B544700EEF22}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -538,10 +538,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5CCD2D-3D10-9346-8A5C-475560897FB9}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,6 +631,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>40</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>